<commit_message>
docs: Test case everlo site file updated
</commit_message>
<xml_diff>
--- a/Test cases for everlo site.xlsx
+++ b/Test cases for everlo site.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="133">
   <si>
     <t>SL</t>
   </si>
@@ -411,6 +411,9 @@
   </si>
   <si>
     <t>https://drive.google.com/file/d/1Pcc4h9nETzJQqaQ60e-83iuH0m-ICw3X/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>System should redirect to create account page.</t>
   </si>
 </sst>
 </file>
@@ -592,24 +595,31 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -620,239 +630,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF1155CC"/>
-          <bgColor rgb="FF1155CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF274E13"/>
-          <bgColor rgb="FF274E13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF1155CC"/>
-          <bgColor rgb="FF1155CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF274E13"/>
-          <bgColor rgb="FF274E13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF1155CC"/>
-          <bgColor rgb="FF1155CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF274E13"/>
-          <bgColor rgb="FF274E13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF1155CC"/>
-          <bgColor rgb="FF1155CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF274E13"/>
-          <bgColor rgb="FF274E13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF1155CC"/>
-          <bgColor rgb="FF1155CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFFFF"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF274E13"/>
-          <bgColor rgb="FF274E13"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FFFFFFFF"/>
@@ -1111,7 +894,7 @@
   <dimension ref="A1:N358"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M56" sqref="M56:M165"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1171,19 +954,19 @@
       <c r="A2" s="34">
         <v>1</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="41" t="s">
         <v>32</v>
       </c>
       <c r="D2" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="29" t="s">
         <v>33</v>
       </c>
       <c r="G2" s="14" t="s">
@@ -1191,7 +974,7 @@
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="14" t="s">
-        <v>15</v>
+        <v>132</v>
       </c>
       <c r="J2" s="7" t="s">
         <v>16</v>
@@ -1202,7 +985,7 @@
     </row>
     <row r="3" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="30"/>
-      <c r="B3" s="37"/>
+      <c r="B3" s="40"/>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
       <c r="E3" s="30"/>
@@ -1225,7 +1008,7 @@
     </row>
     <row r="4" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="30"/>
-      <c r="B4" s="37"/>
+      <c r="B4" s="40"/>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
       <c r="E4" s="30"/>
@@ -1248,7 +1031,7 @@
     </row>
     <row r="5" spans="1:12" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="30"/>
-      <c r="B5" s="37"/>
+      <c r="B5" s="40"/>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
       <c r="E5" s="30"/>
@@ -1274,16 +1057,16 @@
       <c r="B6" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="33" t="s">
         <v>36</v>
       </c>
       <c r="D6" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="36" t="s">
+      <c r="E6" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="33" t="s">
+      <c r="F6" s="29" t="s">
         <v>33</v>
       </c>
       <c r="G6" s="14" t="s">
@@ -1396,16 +1179,16 @@
       <c r="B11" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="31" t="s">
+      <c r="D11" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="32" t="s">
+      <c r="E11" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="33" t="s">
+      <c r="F11" s="29" t="s">
         <v>33</v>
       </c>
       <c r="G11" s="17" t="s">
@@ -1514,16 +1297,16 @@
       <c r="B16" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="29" t="s">
+      <c r="C16" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="31" t="s">
+      <c r="D16" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="E16" s="32" t="s">
+      <c r="E16" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="F16" s="33" t="s">
+      <c r="F16" s="29" t="s">
         <v>33</v>
       </c>
       <c r="G16" s="17" t="s">
@@ -1619,16 +1402,16 @@
       <c r="B21" s="35" t="s">
         <v>77</v>
       </c>
-      <c r="C21" s="29" t="s">
+      <c r="C21" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="D21" s="31" t="s">
+      <c r="D21" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="32" t="s">
+      <c r="E21" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="F21" s="33" t="s">
+      <c r="F21" s="29" t="s">
         <v>59</v>
       </c>
       <c r="G21" s="17" t="s">
@@ -1692,16 +1475,16 @@
       <c r="B26" s="35" t="s">
         <v>78</v>
       </c>
-      <c r="C26" s="29" t="s">
+      <c r="C26" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="D26" s="31" t="s">
+      <c r="D26" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="E26" s="32" t="s">
+      <c r="E26" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="F26" s="33" t="s">
+      <c r="F26" s="29" t="s">
         <v>59</v>
       </c>
       <c r="G26" s="19" t="s">
@@ -1769,16 +1552,16 @@
       <c r="B31" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="C31" s="29" t="s">
+      <c r="C31" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="D31" s="31" t="s">
+      <c r="D31" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="E31" s="32" t="s">
+      <c r="E31" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="F31" s="33" t="s">
+      <c r="F31" s="29" t="s">
         <v>59</v>
       </c>
       <c r="G31" s="19" t="s">
@@ -1849,16 +1632,16 @@
       <c r="B36" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="C36" s="29" t="s">
+      <c r="C36" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="D36" s="31" t="s">
+      <c r="D36" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="E36" s="32" t="s">
+      <c r="E36" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="F36" s="33" t="s">
+      <c r="F36" s="29" t="s">
         <v>98</v>
       </c>
       <c r="G36" s="19" t="s">
@@ -1926,16 +1709,16 @@
       <c r="B41" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="C41" s="29" t="s">
+      <c r="C41" s="33" t="s">
         <v>104</v>
       </c>
-      <c r="D41" s="31" t="s">
+      <c r="D41" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="E41" s="32" t="s">
+      <c r="E41" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="F41" s="33" t="s">
+      <c r="F41" s="29" t="s">
         <v>98</v>
       </c>
       <c r="G41" s="19" t="s">
@@ -2006,16 +1789,16 @@
       <c r="B46" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="C46" s="29" t="s">
+      <c r="C46" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="D46" s="31" t="s">
+      <c r="D46" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="E46" s="32" t="s">
+      <c r="E46" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="F46" s="33" t="s">
+      <c r="F46" s="29" t="s">
         <v>98</v>
       </c>
       <c r="G46" s="19" t="s">
@@ -2101,16 +1884,16 @@
       <c r="B51" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="C51" s="29" t="s">
+      <c r="C51" s="33" t="s">
         <v>124</v>
       </c>
-      <c r="D51" s="31" t="s">
+      <c r="D51" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="E51" s="32" t="s">
+      <c r="E51" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="F51" s="33" t="s">
+      <c r="F51" s="29" t="s">
         <v>59</v>
       </c>
       <c r="G51" s="19" t="s">
@@ -2176,18 +1959,18 @@
         <v>12</v>
       </c>
       <c r="B56" s="35"/>
-      <c r="C56" s="29"/>
-      <c r="D56" s="31"/>
-      <c r="E56" s="32"/>
-      <c r="F56" s="33"/>
-      <c r="G56" s="33"/>
-      <c r="H56" s="32"/>
-      <c r="I56" s="33"/>
-      <c r="J56" s="33"/>
-      <c r="K56" s="32"/>
-      <c r="L56" s="33"/>
-      <c r="M56" s="33"/>
-      <c r="N56" s="33"/>
+      <c r="C56" s="33"/>
+      <c r="D56" s="32"/>
+      <c r="E56" s="31"/>
+      <c r="F56" s="29"/>
+      <c r="G56" s="29"/>
+      <c r="H56" s="31"/>
+      <c r="I56" s="29"/>
+      <c r="J56" s="29"/>
+      <c r="K56" s="31"/>
+      <c r="L56" s="29"/>
+      <c r="M56" s="29"/>
+      <c r="N56" s="29"/>
     </row>
     <row r="57" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="30"/>
@@ -2258,17 +2041,17 @@
         <v>13</v>
       </c>
       <c r="B61" s="35"/>
-      <c r="C61" s="29"/>
-      <c r="D61" s="31"/>
-      <c r="E61" s="32"/>
-      <c r="F61" s="33"/>
-      <c r="G61" s="33"/>
-      <c r="H61" s="32"/>
-      <c r="I61" s="33"/>
-      <c r="J61" s="33"/>
-      <c r="K61" s="32"/>
-      <c r="L61" s="33"/>
-      <c r="M61" s="33"/>
+      <c r="C61" s="33"/>
+      <c r="D61" s="32"/>
+      <c r="E61" s="31"/>
+      <c r="F61" s="29"/>
+      <c r="G61" s="29"/>
+      <c r="H61" s="31"/>
+      <c r="I61" s="29"/>
+      <c r="J61" s="29"/>
+      <c r="K61" s="31"/>
+      <c r="L61" s="29"/>
+      <c r="M61" s="29"/>
     </row>
     <row r="62" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="30"/>
@@ -2335,16 +2118,16 @@
         <v>14</v>
       </c>
       <c r="B66" s="35"/>
-      <c r="C66" s="29"/>
-      <c r="D66" s="31"/>
-      <c r="E66" s="32"/>
-      <c r="F66" s="33"/>
-      <c r="G66" s="33"/>
-      <c r="H66" s="32"/>
-      <c r="I66" s="33"/>
-      <c r="J66" s="33"/>
-      <c r="L66" s="33"/>
-      <c r="M66" s="33"/>
+      <c r="C66" s="33"/>
+      <c r="D66" s="32"/>
+      <c r="E66" s="31"/>
+      <c r="F66" s="29"/>
+      <c r="G66" s="29"/>
+      <c r="H66" s="31"/>
+      <c r="I66" s="29"/>
+      <c r="J66" s="29"/>
+      <c r="L66" s="29"/>
+      <c r="M66" s="29"/>
     </row>
     <row r="67" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="30"/>
@@ -2407,16 +2190,16 @@
         <v>15</v>
       </c>
       <c r="B71" s="35"/>
-      <c r="C71" s="29"/>
-      <c r="D71" s="31"/>
-      <c r="E71" s="32"/>
-      <c r="F71" s="33"/>
-      <c r="G71" s="33"/>
-      <c r="H71" s="32"/>
-      <c r="I71" s="33"/>
-      <c r="J71" s="33"/>
-      <c r="L71" s="33"/>
-      <c r="M71" s="33"/>
+      <c r="C71" s="33"/>
+      <c r="D71" s="32"/>
+      <c r="E71" s="31"/>
+      <c r="F71" s="29"/>
+      <c r="G71" s="29"/>
+      <c r="H71" s="31"/>
+      <c r="I71" s="29"/>
+      <c r="J71" s="29"/>
+      <c r="L71" s="29"/>
+      <c r="M71" s="29"/>
     </row>
     <row r="72" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="30"/>
@@ -2479,16 +2262,16 @@
         <v>16</v>
       </c>
       <c r="B76" s="35"/>
-      <c r="C76" s="29"/>
-      <c r="D76" s="31"/>
-      <c r="E76" s="32"/>
-      <c r="F76" s="33"/>
-      <c r="G76" s="33"/>
-      <c r="H76" s="32"/>
-      <c r="I76" s="33"/>
-      <c r="J76" s="33"/>
-      <c r="L76" s="33"/>
-      <c r="M76" s="33"/>
+      <c r="C76" s="33"/>
+      <c r="D76" s="32"/>
+      <c r="E76" s="31"/>
+      <c r="F76" s="29"/>
+      <c r="G76" s="29"/>
+      <c r="H76" s="31"/>
+      <c r="I76" s="29"/>
+      <c r="J76" s="29"/>
+      <c r="L76" s="29"/>
+      <c r="M76" s="29"/>
     </row>
     <row r="77" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="30"/>
@@ -2551,16 +2334,16 @@
         <v>17</v>
       </c>
       <c r="B81" s="35"/>
-      <c r="C81" s="29"/>
-      <c r="D81" s="31"/>
-      <c r="E81" s="32"/>
-      <c r="F81" s="33"/>
-      <c r="G81" s="33"/>
-      <c r="H81" s="32"/>
-      <c r="I81" s="33"/>
-      <c r="J81" s="33"/>
-      <c r="L81" s="33"/>
-      <c r="M81" s="33"/>
+      <c r="C81" s="33"/>
+      <c r="D81" s="32"/>
+      <c r="E81" s="31"/>
+      <c r="F81" s="29"/>
+      <c r="G81" s="29"/>
+      <c r="H81" s="31"/>
+      <c r="I81" s="29"/>
+      <c r="J81" s="29"/>
+      <c r="L81" s="29"/>
+      <c r="M81" s="29"/>
     </row>
     <row r="82" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="30"/>
@@ -2623,16 +2406,16 @@
         <v>18</v>
       </c>
       <c r="B86" s="35"/>
-      <c r="C86" s="29"/>
-      <c r="D86" s="31"/>
-      <c r="E86" s="32"/>
-      <c r="F86" s="33"/>
-      <c r="G86" s="33"/>
-      <c r="H86" s="32"/>
-      <c r="I86" s="33"/>
-      <c r="J86" s="33"/>
-      <c r="L86" s="33"/>
-      <c r="M86" s="33"/>
+      <c r="C86" s="33"/>
+      <c r="D86" s="32"/>
+      <c r="E86" s="31"/>
+      <c r="F86" s="29"/>
+      <c r="G86" s="29"/>
+      <c r="H86" s="31"/>
+      <c r="I86" s="29"/>
+      <c r="J86" s="29"/>
+      <c r="L86" s="29"/>
+      <c r="M86" s="29"/>
     </row>
     <row r="87" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="30"/>
@@ -2695,16 +2478,16 @@
         <v>19</v>
       </c>
       <c r="B91" s="35"/>
-      <c r="C91" s="29"/>
-      <c r="D91" s="31"/>
-      <c r="E91" s="32"/>
-      <c r="F91" s="33"/>
-      <c r="G91" s="33"/>
-      <c r="H91" s="32"/>
-      <c r="I91" s="33"/>
-      <c r="J91" s="33"/>
-      <c r="L91" s="33"/>
-      <c r="M91" s="33"/>
+      <c r="C91" s="33"/>
+      <c r="D91" s="32"/>
+      <c r="E91" s="31"/>
+      <c r="F91" s="29"/>
+      <c r="G91" s="29"/>
+      <c r="H91" s="31"/>
+      <c r="I91" s="29"/>
+      <c r="J91" s="29"/>
+      <c r="L91" s="29"/>
+      <c r="M91" s="29"/>
     </row>
     <row r="92" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="30"/>
@@ -2767,16 +2550,16 @@
         <v>20</v>
       </c>
       <c r="B96" s="35"/>
-      <c r="C96" s="29"/>
-      <c r="D96" s="31"/>
-      <c r="E96" s="32"/>
-      <c r="F96" s="33"/>
-      <c r="G96" s="33"/>
-      <c r="H96" s="32"/>
-      <c r="I96" s="33"/>
-      <c r="J96" s="33"/>
-      <c r="L96" s="33"/>
-      <c r="M96" s="33"/>
+      <c r="C96" s="33"/>
+      <c r="D96" s="32"/>
+      <c r="E96" s="31"/>
+      <c r="F96" s="29"/>
+      <c r="G96" s="29"/>
+      <c r="H96" s="31"/>
+      <c r="I96" s="29"/>
+      <c r="J96" s="29"/>
+      <c r="L96" s="29"/>
+      <c r="M96" s="29"/>
     </row>
     <row r="97" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="30"/>
@@ -2839,16 +2622,16 @@
         <v>21</v>
       </c>
       <c r="B101" s="35"/>
-      <c r="C101" s="29"/>
-      <c r="D101" s="31"/>
-      <c r="E101" s="32"/>
-      <c r="F101" s="33"/>
-      <c r="G101" s="33"/>
-      <c r="H101" s="32"/>
-      <c r="I101" s="33"/>
-      <c r="J101" s="33"/>
-      <c r="L101" s="33"/>
-      <c r="M101" s="33"/>
+      <c r="C101" s="33"/>
+      <c r="D101" s="32"/>
+      <c r="E101" s="31"/>
+      <c r="F101" s="29"/>
+      <c r="G101" s="29"/>
+      <c r="H101" s="31"/>
+      <c r="I101" s="29"/>
+      <c r="J101" s="29"/>
+      <c r="L101" s="29"/>
+      <c r="M101" s="29"/>
     </row>
     <row r="102" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="30"/>
@@ -2911,16 +2694,16 @@
         <v>22</v>
       </c>
       <c r="B106" s="35"/>
-      <c r="C106" s="29"/>
-      <c r="D106" s="31"/>
-      <c r="E106" s="32"/>
-      <c r="F106" s="33"/>
-      <c r="G106" s="33"/>
-      <c r="H106" s="32"/>
-      <c r="I106" s="33"/>
-      <c r="J106" s="33"/>
-      <c r="L106" s="33"/>
-      <c r="M106" s="33"/>
+      <c r="C106" s="33"/>
+      <c r="D106" s="32"/>
+      <c r="E106" s="31"/>
+      <c r="F106" s="29"/>
+      <c r="G106" s="29"/>
+      <c r="H106" s="31"/>
+      <c r="I106" s="29"/>
+      <c r="J106" s="29"/>
+      <c r="L106" s="29"/>
+      <c r="M106" s="29"/>
     </row>
     <row r="107" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="30"/>
@@ -2983,16 +2766,16 @@
         <v>23</v>
       </c>
       <c r="B111" s="35"/>
-      <c r="C111" s="29"/>
-      <c r="D111" s="31"/>
-      <c r="E111" s="32"/>
-      <c r="F111" s="33"/>
-      <c r="G111" s="33"/>
-      <c r="H111" s="32"/>
-      <c r="I111" s="33"/>
-      <c r="J111" s="33"/>
-      <c r="L111" s="33"/>
-      <c r="M111" s="33"/>
+      <c r="C111" s="33"/>
+      <c r="D111" s="32"/>
+      <c r="E111" s="31"/>
+      <c r="F111" s="29"/>
+      <c r="G111" s="29"/>
+      <c r="H111" s="31"/>
+      <c r="I111" s="29"/>
+      <c r="J111" s="29"/>
+      <c r="L111" s="29"/>
+      <c r="M111" s="29"/>
     </row>
     <row r="112" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="30"/>
@@ -3055,16 +2838,16 @@
         <v>24</v>
       </c>
       <c r="B116" s="35"/>
-      <c r="C116" s="29"/>
-      <c r="D116" s="31"/>
-      <c r="E116" s="32"/>
-      <c r="F116" s="33"/>
-      <c r="G116" s="33"/>
-      <c r="H116" s="32"/>
-      <c r="I116" s="33"/>
-      <c r="J116" s="33"/>
-      <c r="L116" s="33"/>
-      <c r="M116" s="33"/>
+      <c r="C116" s="33"/>
+      <c r="D116" s="32"/>
+      <c r="E116" s="31"/>
+      <c r="F116" s="29"/>
+      <c r="G116" s="29"/>
+      <c r="H116" s="31"/>
+      <c r="I116" s="29"/>
+      <c r="J116" s="29"/>
+      <c r="L116" s="29"/>
+      <c r="M116" s="29"/>
     </row>
     <row r="117" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="30"/>
@@ -3127,16 +2910,16 @@
         <v>25</v>
       </c>
       <c r="B121" s="35"/>
-      <c r="C121" s="29"/>
-      <c r="D121" s="31"/>
-      <c r="E121" s="32"/>
-      <c r="F121" s="33"/>
-      <c r="G121" s="33"/>
-      <c r="H121" s="32"/>
-      <c r="I121" s="33"/>
-      <c r="J121" s="33"/>
-      <c r="L121" s="33"/>
-      <c r="M121" s="33"/>
+      <c r="C121" s="33"/>
+      <c r="D121" s="32"/>
+      <c r="E121" s="31"/>
+      <c r="F121" s="29"/>
+      <c r="G121" s="29"/>
+      <c r="H121" s="31"/>
+      <c r="I121" s="29"/>
+      <c r="J121" s="29"/>
+      <c r="L121" s="29"/>
+      <c r="M121" s="29"/>
     </row>
     <row r="122" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="30"/>
@@ -3199,16 +2982,16 @@
         <v>26</v>
       </c>
       <c r="B126" s="35"/>
-      <c r="C126" s="29"/>
-      <c r="D126" s="31"/>
-      <c r="E126" s="32"/>
-      <c r="F126" s="33"/>
-      <c r="G126" s="33"/>
-      <c r="H126" s="32"/>
-      <c r="I126" s="33"/>
-      <c r="J126" s="33"/>
-      <c r="L126" s="33"/>
-      <c r="M126" s="33"/>
+      <c r="C126" s="33"/>
+      <c r="D126" s="32"/>
+      <c r="E126" s="31"/>
+      <c r="F126" s="29"/>
+      <c r="G126" s="29"/>
+      <c r="H126" s="31"/>
+      <c r="I126" s="29"/>
+      <c r="J126" s="29"/>
+      <c r="L126" s="29"/>
+      <c r="M126" s="29"/>
     </row>
     <row r="127" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="30"/>
@@ -3271,16 +3054,16 @@
         <v>27</v>
       </c>
       <c r="B131" s="35"/>
-      <c r="C131" s="29"/>
-      <c r="D131" s="31"/>
-      <c r="E131" s="32"/>
-      <c r="F131" s="33"/>
-      <c r="G131" s="33"/>
-      <c r="H131" s="32"/>
-      <c r="I131" s="33"/>
-      <c r="J131" s="33"/>
-      <c r="L131" s="33"/>
-      <c r="M131" s="33"/>
+      <c r="C131" s="33"/>
+      <c r="D131" s="32"/>
+      <c r="E131" s="31"/>
+      <c r="F131" s="29"/>
+      <c r="G131" s="29"/>
+      <c r="H131" s="31"/>
+      <c r="I131" s="29"/>
+      <c r="J131" s="29"/>
+      <c r="L131" s="29"/>
+      <c r="M131" s="29"/>
     </row>
     <row r="132" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="30"/>
@@ -3343,16 +3126,16 @@
         <v>28</v>
       </c>
       <c r="B136" s="35"/>
-      <c r="C136" s="29"/>
-      <c r="D136" s="31"/>
-      <c r="E136" s="32"/>
-      <c r="F136" s="33"/>
-      <c r="G136" s="33"/>
-      <c r="H136" s="32"/>
-      <c r="I136" s="33"/>
-      <c r="J136" s="33"/>
-      <c r="L136" s="33"/>
-      <c r="M136" s="33"/>
+      <c r="C136" s="33"/>
+      <c r="D136" s="32"/>
+      <c r="E136" s="31"/>
+      <c r="F136" s="29"/>
+      <c r="G136" s="29"/>
+      <c r="H136" s="31"/>
+      <c r="I136" s="29"/>
+      <c r="J136" s="29"/>
+      <c r="L136" s="29"/>
+      <c r="M136" s="29"/>
     </row>
     <row r="137" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="30"/>
@@ -3415,16 +3198,16 @@
         <v>29</v>
       </c>
       <c r="B141" s="35"/>
-      <c r="C141" s="29"/>
-      <c r="D141" s="31"/>
-      <c r="E141" s="32"/>
-      <c r="F141" s="33"/>
-      <c r="G141" s="33"/>
-      <c r="H141" s="32"/>
-      <c r="I141" s="33"/>
-      <c r="J141" s="33"/>
-      <c r="L141" s="33"/>
-      <c r="M141" s="33"/>
+      <c r="C141" s="33"/>
+      <c r="D141" s="32"/>
+      <c r="E141" s="31"/>
+      <c r="F141" s="29"/>
+      <c r="G141" s="29"/>
+      <c r="H141" s="31"/>
+      <c r="I141" s="29"/>
+      <c r="J141" s="29"/>
+      <c r="L141" s="29"/>
+      <c r="M141" s="29"/>
     </row>
     <row r="142" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="30"/>
@@ -3487,16 +3270,16 @@
         <v>30</v>
       </c>
       <c r="B146" s="35"/>
-      <c r="C146" s="29"/>
-      <c r="D146" s="31"/>
-      <c r="E146" s="32"/>
-      <c r="F146" s="33"/>
-      <c r="G146" s="33"/>
-      <c r="H146" s="32"/>
-      <c r="I146" s="33"/>
-      <c r="J146" s="33"/>
-      <c r="L146" s="33"/>
-      <c r="M146" s="33"/>
+      <c r="C146" s="33"/>
+      <c r="D146" s="32"/>
+      <c r="E146" s="31"/>
+      <c r="F146" s="29"/>
+      <c r="G146" s="29"/>
+      <c r="H146" s="31"/>
+      <c r="I146" s="29"/>
+      <c r="J146" s="29"/>
+      <c r="L146" s="29"/>
+      <c r="M146" s="29"/>
     </row>
     <row r="147" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="30"/>
@@ -3559,16 +3342,16 @@
         <v>31</v>
       </c>
       <c r="B151" s="35"/>
-      <c r="C151" s="29"/>
-      <c r="D151" s="31"/>
-      <c r="E151" s="32"/>
-      <c r="F151" s="33"/>
-      <c r="G151" s="33"/>
-      <c r="H151" s="32"/>
-      <c r="I151" s="33"/>
-      <c r="J151" s="33"/>
-      <c r="L151" s="33"/>
-      <c r="M151" s="33"/>
+      <c r="C151" s="33"/>
+      <c r="D151" s="32"/>
+      <c r="E151" s="31"/>
+      <c r="F151" s="29"/>
+      <c r="G151" s="29"/>
+      <c r="H151" s="31"/>
+      <c r="I151" s="29"/>
+      <c r="J151" s="29"/>
+      <c r="L151" s="29"/>
+      <c r="M151" s="29"/>
     </row>
     <row r="152" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="30"/>
@@ -3628,16 +3411,16 @@
     </row>
     <row r="156" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B156" s="35"/>
-      <c r="C156" s="29"/>
-      <c r="D156" s="31"/>
-      <c r="E156" s="32"/>
-      <c r="F156" s="33"/>
-      <c r="G156" s="33"/>
-      <c r="H156" s="32"/>
-      <c r="I156" s="33"/>
-      <c r="J156" s="33"/>
-      <c r="L156" s="33"/>
-      <c r="M156" s="33"/>
+      <c r="C156" s="33"/>
+      <c r="D156" s="32"/>
+      <c r="E156" s="31"/>
+      <c r="F156" s="29"/>
+      <c r="G156" s="29"/>
+      <c r="H156" s="31"/>
+      <c r="I156" s="29"/>
+      <c r="J156" s="29"/>
+      <c r="L156" s="29"/>
+      <c r="M156" s="29"/>
     </row>
     <row r="157" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B157" s="35"/>
@@ -3692,16 +3475,16 @@
       <c r="M160" s="30"/>
     </row>
     <row r="161" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C161" s="29"/>
-      <c r="D161" s="31"/>
-      <c r="E161" s="32"/>
-      <c r="F161" s="33"/>
-      <c r="G161" s="33"/>
-      <c r="H161" s="32"/>
-      <c r="I161" s="33"/>
-      <c r="J161" s="33"/>
-      <c r="L161" s="33"/>
-      <c r="M161" s="33"/>
+      <c r="C161" s="33"/>
+      <c r="D161" s="32"/>
+      <c r="E161" s="31"/>
+      <c r="F161" s="29"/>
+      <c r="G161" s="29"/>
+      <c r="H161" s="31"/>
+      <c r="I161" s="29"/>
+      <c r="J161" s="29"/>
+      <c r="L161" s="29"/>
+      <c r="M161" s="29"/>
     </row>
     <row r="162" spans="3:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C162" s="30"/>
@@ -3752,44 +3535,44 @@
       <c r="M165" s="30"/>
     </row>
     <row r="354" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A354" s="39" t="s">
+      <c r="A354" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="B354" s="39"/>
-      <c r="C354" s="39"/>
+      <c r="B354" s="38"/>
+      <c r="C354" s="38"/>
     </row>
     <row r="355" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A355" s="40" t="s">
+      <c r="A355" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="B355" s="40"/>
+      <c r="B355" s="36"/>
       <c r="C355" s="11">
         <v>11</v>
       </c>
     </row>
     <row r="356" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A356" s="41" t="s">
+      <c r="A356" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="B356" s="41"/>
+      <c r="B356" s="37"/>
       <c r="C356" s="10">
         <v>9</v>
       </c>
     </row>
     <row r="357" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A357" s="41" t="s">
+      <c r="A357" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="B357" s="41"/>
+      <c r="B357" s="37"/>
       <c r="C357" s="10">
         <v>2</v>
       </c>
     </row>
     <row r="358" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A358" s="40" t="s">
+      <c r="A358" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="B358" s="40"/>
+      <c r="B358" s="36"/>
       <c r="C358" s="12">
         <f>(C356/C355)</f>
         <v>0.81818181818181823</v>
@@ -3797,84 +3580,239 @@
     </row>
   </sheetData>
   <mergeCells count="335">
-    <mergeCell ref="M141:M145"/>
-    <mergeCell ref="M146:M150"/>
-    <mergeCell ref="M151:M155"/>
-    <mergeCell ref="M156:M160"/>
-    <mergeCell ref="M161:M165"/>
-    <mergeCell ref="M116:M120"/>
-    <mergeCell ref="M121:M125"/>
-    <mergeCell ref="M126:M130"/>
-    <mergeCell ref="M131:M135"/>
-    <mergeCell ref="M136:M140"/>
-    <mergeCell ref="M91:M95"/>
-    <mergeCell ref="M96:M100"/>
-    <mergeCell ref="M101:M105"/>
-    <mergeCell ref="M106:M110"/>
-    <mergeCell ref="M111:M115"/>
-    <mergeCell ref="M66:M70"/>
-    <mergeCell ref="M71:M75"/>
-    <mergeCell ref="M76:M80"/>
-    <mergeCell ref="M81:M85"/>
-    <mergeCell ref="M86:M90"/>
-    <mergeCell ref="L141:L145"/>
-    <mergeCell ref="L146:L150"/>
-    <mergeCell ref="L151:L155"/>
-    <mergeCell ref="L156:L160"/>
-    <mergeCell ref="L161:L165"/>
-    <mergeCell ref="L116:L120"/>
-    <mergeCell ref="L121:L125"/>
-    <mergeCell ref="L126:L130"/>
-    <mergeCell ref="L131:L135"/>
-    <mergeCell ref="L136:L140"/>
-    <mergeCell ref="L91:L95"/>
-    <mergeCell ref="L96:L100"/>
-    <mergeCell ref="L101:L105"/>
-    <mergeCell ref="L106:L110"/>
-    <mergeCell ref="L111:L115"/>
-    <mergeCell ref="L66:L70"/>
-    <mergeCell ref="L71:L75"/>
-    <mergeCell ref="L76:L80"/>
-    <mergeCell ref="L81:L85"/>
-    <mergeCell ref="L86:L90"/>
-    <mergeCell ref="K56:K60"/>
-    <mergeCell ref="K61:K65"/>
-    <mergeCell ref="L56:L60"/>
-    <mergeCell ref="M56:M60"/>
-    <mergeCell ref="N56:N60"/>
-    <mergeCell ref="L61:L65"/>
-    <mergeCell ref="M61:M65"/>
-    <mergeCell ref="J141:J145"/>
-    <mergeCell ref="J146:J150"/>
-    <mergeCell ref="J151:J155"/>
-    <mergeCell ref="J156:J160"/>
-    <mergeCell ref="J161:J165"/>
-    <mergeCell ref="J116:J120"/>
-    <mergeCell ref="J121:J125"/>
-    <mergeCell ref="J126:J130"/>
-    <mergeCell ref="J131:J135"/>
-    <mergeCell ref="J136:J140"/>
-    <mergeCell ref="I146:I150"/>
-    <mergeCell ref="I151:I155"/>
-    <mergeCell ref="I156:I160"/>
-    <mergeCell ref="I161:I165"/>
-    <mergeCell ref="J56:J60"/>
-    <mergeCell ref="J61:J65"/>
-    <mergeCell ref="J66:J70"/>
-    <mergeCell ref="J71:J75"/>
-    <mergeCell ref="J76:J80"/>
-    <mergeCell ref="J81:J85"/>
-    <mergeCell ref="J86:J90"/>
-    <mergeCell ref="J91:J95"/>
-    <mergeCell ref="J96:J100"/>
-    <mergeCell ref="J101:J105"/>
-    <mergeCell ref="J106:J110"/>
-    <mergeCell ref="J111:J115"/>
-    <mergeCell ref="I121:I125"/>
-    <mergeCell ref="I126:I130"/>
-    <mergeCell ref="I131:I135"/>
-    <mergeCell ref="I136:I140"/>
-    <mergeCell ref="I141:I145"/>
+    <mergeCell ref="F21:F25"/>
+    <mergeCell ref="E26:E30"/>
+    <mergeCell ref="E31:E35"/>
+    <mergeCell ref="F26:F30"/>
+    <mergeCell ref="F31:F35"/>
+    <mergeCell ref="C51:C55"/>
+    <mergeCell ref="D51:D55"/>
+    <mergeCell ref="E51:E55"/>
+    <mergeCell ref="F51:F55"/>
+    <mergeCell ref="F36:F40"/>
+    <mergeCell ref="F41:F45"/>
+    <mergeCell ref="F46:F50"/>
+    <mergeCell ref="E36:E40"/>
+    <mergeCell ref="E41:E45"/>
+    <mergeCell ref="E46:E50"/>
+    <mergeCell ref="C36:C40"/>
+    <mergeCell ref="C41:C45"/>
+    <mergeCell ref="C46:C50"/>
+    <mergeCell ref="D41:D45"/>
+    <mergeCell ref="D46:D50"/>
+    <mergeCell ref="A26:A30"/>
+    <mergeCell ref="B16:B20"/>
+    <mergeCell ref="B21:B25"/>
+    <mergeCell ref="B26:B30"/>
+    <mergeCell ref="C16:C20"/>
+    <mergeCell ref="C21:C25"/>
+    <mergeCell ref="C26:C30"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="B11:B15"/>
+    <mergeCell ref="C11:C15"/>
+    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="F16:F20"/>
+    <mergeCell ref="D6:D10"/>
+    <mergeCell ref="E6:E10"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="F6:F10"/>
+    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="C6:C10"/>
+    <mergeCell ref="D16:D20"/>
+    <mergeCell ref="B41:B45"/>
+    <mergeCell ref="B46:B50"/>
+    <mergeCell ref="B51:B55"/>
+    <mergeCell ref="C31:C35"/>
+    <mergeCell ref="B96:B100"/>
+    <mergeCell ref="B101:B105"/>
+    <mergeCell ref="B106:B110"/>
+    <mergeCell ref="B111:B115"/>
+    <mergeCell ref="E16:E20"/>
+    <mergeCell ref="D21:D25"/>
+    <mergeCell ref="D26:D30"/>
+    <mergeCell ref="D31:D35"/>
+    <mergeCell ref="D36:D40"/>
+    <mergeCell ref="E21:E25"/>
+    <mergeCell ref="A355:B355"/>
+    <mergeCell ref="A356:B356"/>
+    <mergeCell ref="A357:B357"/>
+    <mergeCell ref="A358:B358"/>
+    <mergeCell ref="F11:F15"/>
+    <mergeCell ref="D11:D15"/>
+    <mergeCell ref="E11:E15"/>
+    <mergeCell ref="A56:A60"/>
+    <mergeCell ref="B56:B60"/>
+    <mergeCell ref="B61:B65"/>
+    <mergeCell ref="B66:B70"/>
+    <mergeCell ref="B71:B75"/>
+    <mergeCell ref="B76:B80"/>
+    <mergeCell ref="B81:B85"/>
+    <mergeCell ref="B86:B90"/>
+    <mergeCell ref="B91:B95"/>
+    <mergeCell ref="A354:C354"/>
+    <mergeCell ref="A31:A35"/>
+    <mergeCell ref="A36:A40"/>
+    <mergeCell ref="A41:A45"/>
+    <mergeCell ref="A46:A50"/>
+    <mergeCell ref="A51:A55"/>
+    <mergeCell ref="B31:B35"/>
+    <mergeCell ref="B36:B40"/>
+    <mergeCell ref="B156:B160"/>
+    <mergeCell ref="A61:A65"/>
+    <mergeCell ref="A66:A70"/>
+    <mergeCell ref="A71:A75"/>
+    <mergeCell ref="A76:A80"/>
+    <mergeCell ref="A81:A85"/>
+    <mergeCell ref="A86:A90"/>
+    <mergeCell ref="A91:A95"/>
+    <mergeCell ref="A96:A100"/>
+    <mergeCell ref="A101:A105"/>
+    <mergeCell ref="A106:A110"/>
+    <mergeCell ref="A111:A115"/>
+    <mergeCell ref="A116:A120"/>
+    <mergeCell ref="B116:B120"/>
+    <mergeCell ref="B121:B125"/>
+    <mergeCell ref="B126:B130"/>
+    <mergeCell ref="B131:B135"/>
+    <mergeCell ref="B136:B140"/>
+    <mergeCell ref="A146:A150"/>
+    <mergeCell ref="A151:A155"/>
+    <mergeCell ref="C56:C60"/>
+    <mergeCell ref="C61:C65"/>
+    <mergeCell ref="C66:C70"/>
+    <mergeCell ref="C71:C75"/>
+    <mergeCell ref="C76:C80"/>
+    <mergeCell ref="C81:C85"/>
+    <mergeCell ref="C86:C90"/>
+    <mergeCell ref="C91:C95"/>
+    <mergeCell ref="C96:C100"/>
+    <mergeCell ref="C101:C105"/>
+    <mergeCell ref="C106:C110"/>
+    <mergeCell ref="C111:C115"/>
+    <mergeCell ref="C116:C120"/>
+    <mergeCell ref="C121:C125"/>
+    <mergeCell ref="A121:A125"/>
+    <mergeCell ref="A126:A130"/>
+    <mergeCell ref="A131:A135"/>
+    <mergeCell ref="A136:A140"/>
+    <mergeCell ref="A141:A145"/>
+    <mergeCell ref="B141:B145"/>
+    <mergeCell ref="B146:B150"/>
+    <mergeCell ref="B151:B155"/>
+    <mergeCell ref="C151:C155"/>
+    <mergeCell ref="C156:C160"/>
+    <mergeCell ref="C161:C165"/>
+    <mergeCell ref="D56:D60"/>
+    <mergeCell ref="D61:D65"/>
+    <mergeCell ref="D66:D70"/>
+    <mergeCell ref="D71:D75"/>
+    <mergeCell ref="D76:D80"/>
+    <mergeCell ref="D81:D85"/>
+    <mergeCell ref="D86:D90"/>
+    <mergeCell ref="D91:D95"/>
+    <mergeCell ref="D96:D100"/>
+    <mergeCell ref="D101:D105"/>
+    <mergeCell ref="D106:D110"/>
+    <mergeCell ref="D111:D115"/>
+    <mergeCell ref="D116:D120"/>
+    <mergeCell ref="C126:C130"/>
+    <mergeCell ref="C131:C135"/>
+    <mergeCell ref="C136:C140"/>
+    <mergeCell ref="C141:C145"/>
+    <mergeCell ref="C146:C150"/>
+    <mergeCell ref="D146:D150"/>
+    <mergeCell ref="D151:D155"/>
+    <mergeCell ref="D156:D160"/>
+    <mergeCell ref="D161:D165"/>
+    <mergeCell ref="E56:E60"/>
+    <mergeCell ref="E61:E65"/>
+    <mergeCell ref="E66:E70"/>
+    <mergeCell ref="E71:E75"/>
+    <mergeCell ref="E76:E80"/>
+    <mergeCell ref="E81:E85"/>
+    <mergeCell ref="E86:E90"/>
+    <mergeCell ref="E91:E95"/>
+    <mergeCell ref="E96:E100"/>
+    <mergeCell ref="E101:E105"/>
+    <mergeCell ref="E106:E110"/>
+    <mergeCell ref="E111:E115"/>
+    <mergeCell ref="D121:D125"/>
+    <mergeCell ref="D126:D130"/>
+    <mergeCell ref="D131:D135"/>
+    <mergeCell ref="D136:D140"/>
+    <mergeCell ref="D141:D145"/>
+    <mergeCell ref="F146:F150"/>
+    <mergeCell ref="E141:E145"/>
+    <mergeCell ref="E146:E150"/>
+    <mergeCell ref="F56:F60"/>
+    <mergeCell ref="F66:F70"/>
+    <mergeCell ref="F71:F75"/>
+    <mergeCell ref="F76:F80"/>
+    <mergeCell ref="F81:F85"/>
+    <mergeCell ref="F86:F90"/>
+    <mergeCell ref="F91:F95"/>
+    <mergeCell ref="F96:F100"/>
+    <mergeCell ref="F101:F105"/>
+    <mergeCell ref="F106:F110"/>
+    <mergeCell ref="F111:F115"/>
+    <mergeCell ref="F116:F120"/>
+    <mergeCell ref="F121:F125"/>
+    <mergeCell ref="E116:E120"/>
+    <mergeCell ref="E121:E125"/>
+    <mergeCell ref="E126:E130"/>
+    <mergeCell ref="E131:E135"/>
+    <mergeCell ref="E136:E140"/>
+    <mergeCell ref="G56:G60"/>
+    <mergeCell ref="G61:G65"/>
+    <mergeCell ref="G66:G70"/>
+    <mergeCell ref="G71:G75"/>
+    <mergeCell ref="G76:G80"/>
+    <mergeCell ref="F126:F130"/>
+    <mergeCell ref="F131:F135"/>
+    <mergeCell ref="F136:F140"/>
+    <mergeCell ref="F141:F145"/>
+    <mergeCell ref="F61:F65"/>
+    <mergeCell ref="G106:G110"/>
+    <mergeCell ref="G111:G115"/>
+    <mergeCell ref="G116:G120"/>
+    <mergeCell ref="G121:G125"/>
+    <mergeCell ref="G126:G130"/>
+    <mergeCell ref="G81:G85"/>
+    <mergeCell ref="G86:G90"/>
+    <mergeCell ref="G91:G95"/>
+    <mergeCell ref="G96:G100"/>
+    <mergeCell ref="G101:G105"/>
+    <mergeCell ref="H131:H135"/>
+    <mergeCell ref="H136:H140"/>
+    <mergeCell ref="H141:H145"/>
+    <mergeCell ref="H146:H150"/>
+    <mergeCell ref="G151:G155"/>
+    <mergeCell ref="G156:G160"/>
+    <mergeCell ref="H56:H60"/>
+    <mergeCell ref="H61:H65"/>
+    <mergeCell ref="H66:H70"/>
+    <mergeCell ref="H71:H75"/>
+    <mergeCell ref="H76:H80"/>
+    <mergeCell ref="H81:H85"/>
+    <mergeCell ref="H86:H90"/>
+    <mergeCell ref="H91:H95"/>
+    <mergeCell ref="H96:H100"/>
+    <mergeCell ref="H101:H105"/>
+    <mergeCell ref="H106:H110"/>
+    <mergeCell ref="H111:H115"/>
+    <mergeCell ref="H116:H120"/>
+    <mergeCell ref="H121:H125"/>
+    <mergeCell ref="G131:G135"/>
+    <mergeCell ref="G136:G140"/>
+    <mergeCell ref="G141:G145"/>
+    <mergeCell ref="G146:G150"/>
     <mergeCell ref="E151:E155"/>
     <mergeCell ref="E156:E160"/>
     <mergeCell ref="E161:E165"/>
@@ -3899,257 +3837,102 @@
     <mergeCell ref="F156:F160"/>
     <mergeCell ref="F161:F165"/>
     <mergeCell ref="H126:H130"/>
-    <mergeCell ref="H131:H135"/>
-    <mergeCell ref="H136:H140"/>
-    <mergeCell ref="H141:H145"/>
-    <mergeCell ref="H146:H150"/>
-    <mergeCell ref="G151:G155"/>
-    <mergeCell ref="G156:G160"/>
-    <mergeCell ref="H56:H60"/>
-    <mergeCell ref="H61:H65"/>
-    <mergeCell ref="H66:H70"/>
-    <mergeCell ref="H71:H75"/>
-    <mergeCell ref="H76:H80"/>
-    <mergeCell ref="H81:H85"/>
-    <mergeCell ref="H86:H90"/>
-    <mergeCell ref="H91:H95"/>
-    <mergeCell ref="H96:H100"/>
-    <mergeCell ref="H101:H105"/>
-    <mergeCell ref="H106:H110"/>
-    <mergeCell ref="H111:H115"/>
-    <mergeCell ref="H116:H120"/>
-    <mergeCell ref="H121:H125"/>
-    <mergeCell ref="G131:G135"/>
-    <mergeCell ref="G136:G140"/>
-    <mergeCell ref="G141:G145"/>
-    <mergeCell ref="G146:G150"/>
-    <mergeCell ref="F61:F65"/>
-    <mergeCell ref="G106:G110"/>
-    <mergeCell ref="G111:G115"/>
-    <mergeCell ref="G116:G120"/>
-    <mergeCell ref="G121:G125"/>
-    <mergeCell ref="G126:G130"/>
-    <mergeCell ref="G81:G85"/>
-    <mergeCell ref="G86:G90"/>
-    <mergeCell ref="G91:G95"/>
-    <mergeCell ref="G96:G100"/>
-    <mergeCell ref="G101:G105"/>
-    <mergeCell ref="G56:G60"/>
-    <mergeCell ref="G61:G65"/>
-    <mergeCell ref="G66:G70"/>
-    <mergeCell ref="G71:G75"/>
-    <mergeCell ref="G76:G80"/>
-    <mergeCell ref="F126:F130"/>
-    <mergeCell ref="F131:F135"/>
-    <mergeCell ref="F136:F140"/>
-    <mergeCell ref="F141:F145"/>
-    <mergeCell ref="F146:F150"/>
-    <mergeCell ref="E141:E145"/>
-    <mergeCell ref="E146:E150"/>
-    <mergeCell ref="F56:F60"/>
-    <mergeCell ref="F66:F70"/>
-    <mergeCell ref="F71:F75"/>
-    <mergeCell ref="F76:F80"/>
-    <mergeCell ref="F81:F85"/>
-    <mergeCell ref="F86:F90"/>
-    <mergeCell ref="F91:F95"/>
-    <mergeCell ref="F96:F100"/>
-    <mergeCell ref="F101:F105"/>
-    <mergeCell ref="F106:F110"/>
-    <mergeCell ref="F111:F115"/>
-    <mergeCell ref="F116:F120"/>
-    <mergeCell ref="F121:F125"/>
-    <mergeCell ref="E116:E120"/>
-    <mergeCell ref="E121:E125"/>
-    <mergeCell ref="E126:E130"/>
-    <mergeCell ref="E131:E135"/>
-    <mergeCell ref="E136:E140"/>
-    <mergeCell ref="D146:D150"/>
-    <mergeCell ref="D151:D155"/>
-    <mergeCell ref="D156:D160"/>
-    <mergeCell ref="D161:D165"/>
-    <mergeCell ref="E56:E60"/>
-    <mergeCell ref="E61:E65"/>
-    <mergeCell ref="E66:E70"/>
-    <mergeCell ref="E71:E75"/>
-    <mergeCell ref="E76:E80"/>
-    <mergeCell ref="E81:E85"/>
-    <mergeCell ref="E86:E90"/>
-    <mergeCell ref="E91:E95"/>
-    <mergeCell ref="E96:E100"/>
-    <mergeCell ref="E101:E105"/>
-    <mergeCell ref="E106:E110"/>
-    <mergeCell ref="E111:E115"/>
-    <mergeCell ref="D121:D125"/>
-    <mergeCell ref="D126:D130"/>
-    <mergeCell ref="D131:D135"/>
-    <mergeCell ref="D136:D140"/>
-    <mergeCell ref="D141:D145"/>
-    <mergeCell ref="C151:C155"/>
-    <mergeCell ref="C156:C160"/>
-    <mergeCell ref="C161:C165"/>
-    <mergeCell ref="D56:D60"/>
-    <mergeCell ref="D61:D65"/>
-    <mergeCell ref="D66:D70"/>
-    <mergeCell ref="D71:D75"/>
-    <mergeCell ref="D76:D80"/>
-    <mergeCell ref="D81:D85"/>
-    <mergeCell ref="D86:D90"/>
-    <mergeCell ref="D91:D95"/>
-    <mergeCell ref="D96:D100"/>
-    <mergeCell ref="D101:D105"/>
-    <mergeCell ref="D106:D110"/>
-    <mergeCell ref="D111:D115"/>
-    <mergeCell ref="D116:D120"/>
-    <mergeCell ref="C126:C130"/>
-    <mergeCell ref="C131:C135"/>
-    <mergeCell ref="C136:C140"/>
-    <mergeCell ref="C141:C145"/>
-    <mergeCell ref="C146:C150"/>
-    <mergeCell ref="A146:A150"/>
-    <mergeCell ref="A151:A155"/>
-    <mergeCell ref="C56:C60"/>
-    <mergeCell ref="C61:C65"/>
-    <mergeCell ref="C66:C70"/>
-    <mergeCell ref="C71:C75"/>
-    <mergeCell ref="C76:C80"/>
-    <mergeCell ref="C81:C85"/>
-    <mergeCell ref="C86:C90"/>
-    <mergeCell ref="C91:C95"/>
-    <mergeCell ref="C96:C100"/>
-    <mergeCell ref="C101:C105"/>
-    <mergeCell ref="C106:C110"/>
-    <mergeCell ref="C111:C115"/>
-    <mergeCell ref="C116:C120"/>
-    <mergeCell ref="C121:C125"/>
-    <mergeCell ref="A121:A125"/>
-    <mergeCell ref="A126:A130"/>
-    <mergeCell ref="A131:A135"/>
-    <mergeCell ref="A136:A140"/>
-    <mergeCell ref="A141:A145"/>
-    <mergeCell ref="B141:B145"/>
-    <mergeCell ref="B146:B150"/>
-    <mergeCell ref="B151:B155"/>
-    <mergeCell ref="B156:B160"/>
-    <mergeCell ref="A61:A65"/>
-    <mergeCell ref="A66:A70"/>
-    <mergeCell ref="A71:A75"/>
-    <mergeCell ref="A76:A80"/>
-    <mergeCell ref="A81:A85"/>
-    <mergeCell ref="A86:A90"/>
-    <mergeCell ref="A91:A95"/>
-    <mergeCell ref="A96:A100"/>
-    <mergeCell ref="A101:A105"/>
-    <mergeCell ref="A106:A110"/>
-    <mergeCell ref="A111:A115"/>
-    <mergeCell ref="A116:A120"/>
-    <mergeCell ref="B116:B120"/>
-    <mergeCell ref="B121:B125"/>
-    <mergeCell ref="B126:B130"/>
-    <mergeCell ref="B131:B135"/>
-    <mergeCell ref="B136:B140"/>
-    <mergeCell ref="A355:B355"/>
-    <mergeCell ref="A356:B356"/>
-    <mergeCell ref="A357:B357"/>
-    <mergeCell ref="A358:B358"/>
-    <mergeCell ref="F11:F15"/>
-    <mergeCell ref="D11:D15"/>
-    <mergeCell ref="E11:E15"/>
-    <mergeCell ref="A56:A60"/>
-    <mergeCell ref="B56:B60"/>
-    <mergeCell ref="B61:B65"/>
-    <mergeCell ref="B66:B70"/>
-    <mergeCell ref="B71:B75"/>
-    <mergeCell ref="B76:B80"/>
-    <mergeCell ref="B81:B85"/>
-    <mergeCell ref="B86:B90"/>
-    <mergeCell ref="B91:B95"/>
-    <mergeCell ref="A354:C354"/>
-    <mergeCell ref="A31:A35"/>
-    <mergeCell ref="A36:A40"/>
-    <mergeCell ref="A41:A45"/>
-    <mergeCell ref="A46:A50"/>
-    <mergeCell ref="A51:A55"/>
-    <mergeCell ref="B31:B35"/>
-    <mergeCell ref="B36:B40"/>
-    <mergeCell ref="B41:B45"/>
-    <mergeCell ref="B46:B50"/>
-    <mergeCell ref="B51:B55"/>
-    <mergeCell ref="C31:C35"/>
-    <mergeCell ref="B96:B100"/>
-    <mergeCell ref="B101:B105"/>
-    <mergeCell ref="B106:B110"/>
-    <mergeCell ref="B111:B115"/>
-    <mergeCell ref="E16:E20"/>
-    <mergeCell ref="F16:F20"/>
-    <mergeCell ref="D6:D10"/>
-    <mergeCell ref="E6:E10"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="D2:D5"/>
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="F2:F5"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="F6:F10"/>
-    <mergeCell ref="B6:B10"/>
-    <mergeCell ref="C6:C10"/>
-    <mergeCell ref="A26:A30"/>
-    <mergeCell ref="B16:B20"/>
-    <mergeCell ref="B21:B25"/>
-    <mergeCell ref="B26:B30"/>
-    <mergeCell ref="C16:C20"/>
-    <mergeCell ref="C21:C25"/>
-    <mergeCell ref="C26:C30"/>
-    <mergeCell ref="A11:A15"/>
-    <mergeCell ref="B11:B15"/>
-    <mergeCell ref="C11:C15"/>
-    <mergeCell ref="A16:A20"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="D16:D20"/>
-    <mergeCell ref="D21:D25"/>
-    <mergeCell ref="D26:D30"/>
-    <mergeCell ref="D31:D35"/>
-    <mergeCell ref="D36:D40"/>
-    <mergeCell ref="E21:E25"/>
-    <mergeCell ref="F21:F25"/>
-    <mergeCell ref="E26:E30"/>
-    <mergeCell ref="E31:E35"/>
-    <mergeCell ref="F26:F30"/>
-    <mergeCell ref="F31:F35"/>
-    <mergeCell ref="C51:C55"/>
-    <mergeCell ref="D51:D55"/>
-    <mergeCell ref="E51:E55"/>
-    <mergeCell ref="F51:F55"/>
-    <mergeCell ref="F36:F40"/>
-    <mergeCell ref="F41:F45"/>
-    <mergeCell ref="F46:F50"/>
-    <mergeCell ref="E36:E40"/>
-    <mergeCell ref="E41:E45"/>
-    <mergeCell ref="E46:E50"/>
-    <mergeCell ref="C36:C40"/>
-    <mergeCell ref="C41:C45"/>
-    <mergeCell ref="C46:C50"/>
-    <mergeCell ref="D41:D45"/>
-    <mergeCell ref="D46:D50"/>
+    <mergeCell ref="J151:J155"/>
+    <mergeCell ref="J156:J160"/>
+    <mergeCell ref="J161:J165"/>
+    <mergeCell ref="J116:J120"/>
+    <mergeCell ref="J121:J125"/>
+    <mergeCell ref="J126:J130"/>
+    <mergeCell ref="J131:J135"/>
+    <mergeCell ref="J136:J140"/>
+    <mergeCell ref="I146:I150"/>
+    <mergeCell ref="I151:I155"/>
+    <mergeCell ref="I156:I160"/>
+    <mergeCell ref="I161:I165"/>
+    <mergeCell ref="I121:I125"/>
+    <mergeCell ref="I126:I130"/>
+    <mergeCell ref="I131:I135"/>
+    <mergeCell ref="I136:I140"/>
+    <mergeCell ref="I141:I145"/>
+    <mergeCell ref="K56:K60"/>
+    <mergeCell ref="K61:K65"/>
+    <mergeCell ref="L56:L60"/>
+    <mergeCell ref="M56:M60"/>
+    <mergeCell ref="N56:N60"/>
+    <mergeCell ref="L61:L65"/>
+    <mergeCell ref="M61:M65"/>
+    <mergeCell ref="J141:J145"/>
+    <mergeCell ref="J146:J150"/>
+    <mergeCell ref="J56:J60"/>
+    <mergeCell ref="J61:J65"/>
+    <mergeCell ref="J66:J70"/>
+    <mergeCell ref="J71:J75"/>
+    <mergeCell ref="J76:J80"/>
+    <mergeCell ref="J81:J85"/>
+    <mergeCell ref="J86:J90"/>
+    <mergeCell ref="J91:J95"/>
+    <mergeCell ref="J96:J100"/>
+    <mergeCell ref="J101:J105"/>
+    <mergeCell ref="J106:J110"/>
+    <mergeCell ref="J111:J115"/>
+    <mergeCell ref="L91:L95"/>
+    <mergeCell ref="L96:L100"/>
+    <mergeCell ref="L101:L105"/>
+    <mergeCell ref="L106:L110"/>
+    <mergeCell ref="L111:L115"/>
+    <mergeCell ref="L66:L70"/>
+    <mergeCell ref="L71:L75"/>
+    <mergeCell ref="L76:L80"/>
+    <mergeCell ref="L81:L85"/>
+    <mergeCell ref="L86:L90"/>
+    <mergeCell ref="L141:L145"/>
+    <mergeCell ref="L146:L150"/>
+    <mergeCell ref="L151:L155"/>
+    <mergeCell ref="L156:L160"/>
+    <mergeCell ref="L161:L165"/>
+    <mergeCell ref="L116:L120"/>
+    <mergeCell ref="L121:L125"/>
+    <mergeCell ref="L126:L130"/>
+    <mergeCell ref="L131:L135"/>
+    <mergeCell ref="L136:L140"/>
+    <mergeCell ref="M91:M95"/>
+    <mergeCell ref="M96:M100"/>
+    <mergeCell ref="M101:M105"/>
+    <mergeCell ref="M106:M110"/>
+    <mergeCell ref="M111:M115"/>
+    <mergeCell ref="M66:M70"/>
+    <mergeCell ref="M71:M75"/>
+    <mergeCell ref="M76:M80"/>
+    <mergeCell ref="M81:M85"/>
+    <mergeCell ref="M86:M90"/>
+    <mergeCell ref="M141:M145"/>
+    <mergeCell ref="M146:M150"/>
+    <mergeCell ref="M151:M155"/>
+    <mergeCell ref="M156:M160"/>
+    <mergeCell ref="M161:M165"/>
+    <mergeCell ref="M116:M120"/>
+    <mergeCell ref="M121:M125"/>
+    <mergeCell ref="M126:M130"/>
+    <mergeCell ref="M131:M135"/>
+    <mergeCell ref="M136:M140"/>
   </mergeCells>
   <conditionalFormatting sqref="K2:K55">
-    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH(("Pass"),(K2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K55">
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="Fail">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH(("Fail"),(K2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K55">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Skip">
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="Skip">
       <formula>NOT(ISERROR(SEARCH(("Skip"),(K2))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K55">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Not Executed">
+    <cfRule type="containsText" dxfId="0" priority="5" operator="containsText" text="Not Executed">
       <formula>NOT(ISERROR(SEARCH(("Not Executed"),(K2))))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>